<commit_message>
Adjust for run_simulation.sh script mer 18 gen 2023, 20:18:35, CET
</commit_message>
<xml_diff>
--- a/simulations.xlsx
+++ b/simulations.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>Machine</t>
   </si>
@@ -70,9 +70,6 @@
   </si>
   <si>
     <t>0.035</t>
-  </si>
-  <si>
-    <t>4/100</t>
   </si>
   <si>
     <t>both</t>
@@ -192,14 +189,14 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="2"/>
-        <bgColor indexed="2"/>
+        <fgColor rgb="FF92D050"/>
+        <bgColor rgb="FF92D050"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
-        <bgColor rgb="FF92D050"/>
+        <fgColor indexed="2"/>
+        <bgColor indexed="2"/>
       </patternFill>
     </fill>
   </fills>
@@ -216,7 +213,7 @@
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf fontId="1" fillId="2" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="11">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="2" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -239,16 +236,10 @@
     <xf fontId="2" fillId="6" borderId="0" numFmtId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf fontId="2" fillId="7" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf fontId="2" fillId="3" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf fontId="2" fillId="8" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf fontId="2" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf fontId="2" fillId="7" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf fontId="2" fillId="8" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -762,7 +753,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView zoomScale="100" workbookViewId="0">
+    <sheetView topLeftCell="F1" zoomScale="100" workbookViewId="0">
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -865,20 +856,18 @@
         <v>18</v>
       </c>
       <c r="I3" s="1">
-        <v>96</v>
-      </c>
-      <c r="J3" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="J3" s="1">
+        <v>0</v>
+      </c>
+      <c r="M3" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="M3" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="N3" s="8">
-        <v>1</v>
-      </c>
+      <c r="N3" s="1"/>
     </row>
     <row r="4" ht="14.25">
-      <c r="A4" s="9"/>
+      <c r="A4" s="8"/>
       <c r="B4" s="1">
         <v>24</v>
       </c>
@@ -903,15 +892,18 @@
       <c r="I4" s="1">
         <v>0</v>
       </c>
-      <c r="J4" s="10">
+      <c r="J4" s="9">
         <v>0</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
+      </c>
+      <c r="N4" s="10">
+        <v>25</v>
       </c>
     </row>
     <row r="5" ht="14.25">
-      <c r="A5" s="9"/>
+      <c r="A5" s="8"/>
       <c r="B5" s="1">
         <v>32</v>
       </c>
@@ -936,15 +928,15 @@
       <c r="I5" s="1">
         <v>0</v>
       </c>
-      <c r="J5" s="10">
+      <c r="J5" s="9">
         <v>0</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" ht="14.25">
-      <c r="A6" s="9"/>
+      <c r="A6" s="8"/>
       <c r="B6" s="1">
         <v>48</v>
       </c>
@@ -973,32 +965,32 @@
         <v>0</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" ht="14.25">
-      <c r="A7" s="9"/>
+      <c r="A7" s="8"/>
       <c r="B7" s="1"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="11"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
-      <c r="H7" s="11"/>
-      <c r="I7" s="11"/>
-      <c r="J7" s="11"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
     </row>
     <row r="8" s="5" customFormat="1" ht="15">
       <c r="A8" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B8" s="5"/>
       <c r="F8" s="5"/>
       <c r="G8" s="5"/>
     </row>
     <row r="9" ht="14.25">
-      <c r="A9" s="9" t="s">
-        <v>22</v>
+      <c r="A9" s="8" t="s">
+        <v>21</v>
       </c>
       <c r="B9" s="1">
         <v>18</v>
@@ -1024,15 +1016,15 @@
       <c r="I9" s="1">
         <v>0</v>
       </c>
-      <c r="J9" s="10">
+      <c r="J9" s="9">
         <v>0</v>
       </c>
       <c r="M9" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" ht="14.25">
-      <c r="A10" s="9"/>
+      <c r="A10" s="8"/>
       <c r="B10" s="1">
         <v>24</v>
       </c>
@@ -1057,24 +1049,24 @@
       <c r="I10" s="1">
         <v>0</v>
       </c>
-      <c r="J10" s="10">
+      <c r="J10" s="9">
         <v>0</v>
       </c>
       <c r="K10" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="L10" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="L10" s="1" t="s">
-        <v>24</v>
-      </c>
       <c r="M10" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="N10" s="8">
+        <v>19</v>
+      </c>
+      <c r="N10" s="10">
         <v>25</v>
       </c>
     </row>
     <row r="11" ht="14.25">
-      <c r="A11" s="9"/>
+      <c r="A11" s="8"/>
       <c r="B11" s="1">
         <v>32</v>
       </c>
@@ -1099,15 +1091,15 @@
       <c r="I11" s="1">
         <v>0</v>
       </c>
-      <c r="J11" s="10">
+      <c r="J11" s="9">
         <v>0</v>
       </c>
       <c r="M11" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="12" ht="14.25">
-      <c r="A12" s="9"/>
+      <c r="A12" s="8"/>
       <c r="B12" s="1">
         <v>48</v>
       </c>
@@ -1132,28 +1124,28 @@
       <c r="I12" s="1">
         <v>0</v>
       </c>
-      <c r="J12" s="10">
+      <c r="J12" s="9">
         <v>0</v>
       </c>
       <c r="M12" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="13" ht="14.25">
-      <c r="A13" s="9"/>
+      <c r="A13" s="8"/>
       <c r="B13" s="1"/>
-      <c r="C13" s="11"/>
-      <c r="D13" s="11"/>
-      <c r="E13" s="11"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
-      <c r="H13" s="11"/>
-      <c r="I13" s="11"/>
-      <c r="J13" s="12"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="9"/>
     </row>
     <row r="14" s="5" customFormat="1" ht="15">
       <c r="A14" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
@@ -1166,8 +1158,8 @@
       <c r="J14" s="5"/>
     </row>
     <row r="15" ht="14.25">
-      <c r="A15" s="9" t="s">
-        <v>26</v>
+      <c r="A15" s="8" t="s">
+        <v>25</v>
       </c>
       <c r="B15" s="1">
         <v>96</v>
@@ -1193,24 +1185,24 @@
       <c r="I15" s="1">
         <v>0</v>
       </c>
-      <c r="J15" s="10">
+      <c r="J15" s="9">
         <v>0</v>
       </c>
       <c r="K15" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="L15" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="L15" s="1" t="s">
-        <v>28</v>
-      </c>
       <c r="M15" s="1">
         <v>0</v>
       </c>
-      <c r="N15" s="8">
+      <c r="N15" s="10">
         <v>10</v>
       </c>
     </row>
     <row r="16" ht="14.25">
-      <c r="A16" s="9"/>
+      <c r="A16" s="8"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
@@ -1219,19 +1211,19 @@
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
-      <c r="J16" s="10"/>
+      <c r="J16" s="9"/>
     </row>
     <row r="17" s="5" customFormat="1" ht="15">
       <c r="A17" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B17" s="5"/>
       <c r="F17" s="5"/>
       <c r="G17" s="5"/>
     </row>
     <row r="18" ht="14.25">
-      <c r="A18" s="9" t="s">
-        <v>30</v>
+      <c r="A18" s="8" t="s">
+        <v>29</v>
       </c>
       <c r="B18" s="1">
         <v>62</v>
@@ -1257,18 +1249,18 @@
       <c r="I18" s="1">
         <v>0</v>
       </c>
-      <c r="J18" s="10">
+      <c r="J18" s="9">
         <v>0</v>
       </c>
       <c r="M18" s="1">
         <v>0</v>
       </c>
-      <c r="N18" s="8">
+      <c r="N18" s="10">
         <v>10</v>
       </c>
     </row>
     <row r="19" ht="14.25">
-      <c r="A19" s="9"/>
+      <c r="A19" s="8"/>
       <c r="B19" s="1">
         <v>120</v>
       </c>
@@ -1293,21 +1285,21 @@
       <c r="I19" s="1">
         <v>0</v>
       </c>
-      <c r="J19" s="10">
+      <c r="J19" s="9">
         <v>0</v>
       </c>
       <c r="K19" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="L19" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="L19" s="1" t="s">
-        <v>32</v>
-      </c>
       <c r="M19" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="20" ht="14.25">
-      <c r="A20" s="9"/>
+      <c r="A20" s="8"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
@@ -1316,10 +1308,10 @@
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
-      <c r="J20" s="10"/>
+      <c r="J20" s="9"/>
     </row>
     <row r="21" ht="14.25">
-      <c r="A21" s="9"/>
+      <c r="A21" s="8"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
@@ -1328,18 +1320,18 @@
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
-      <c r="J21" s="10"/>
+      <c r="J21" s="9"/>
     </row>
     <row r="22" s="5" customFormat="1" ht="15">
       <c r="A22" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B22" s="5"/>
       <c r="F22" s="5"/>
     </row>
     <row r="23" ht="14.25">
-      <c r="A23" s="9" t="s">
-        <v>34</v>
+      <c r="A23" s="8" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="25" ht="14.25">

</xml_diff>

<commit_message>
Updated simulation table gio 19 gen 2023, 16:20:52, CET
</commit_message>
<xml_diff>
--- a/simulations.xlsx
+++ b/simulations.xlsx
@@ -121,7 +121,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <name val="Calibri"/>
       <color theme="1"/>
@@ -146,6 +146,12 @@
       <b/>
       <i/>
       <color theme="1"/>
+      <sz val="11.000000"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <b/>
       <sz val="11.000000"/>
       <scheme val="minor"/>
     </font>
@@ -189,14 +195,14 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
-        <bgColor rgb="FF92D050"/>
+        <fgColor rgb="FF0070C0"/>
+        <bgColor rgb="FF0070C0"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="2"/>
-        <bgColor indexed="2"/>
+        <fgColor rgb="FF92D050"/>
+        <bgColor rgb="FF92D050"/>
       </patternFill>
     </fill>
   </fills>
@@ -213,7 +219,7 @@
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf fontId="1" fillId="2" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="2" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -236,13 +242,16 @@
     <xf fontId="2" fillId="6" borderId="0" numFmtId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf fontId="2" fillId="7" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf fontId="2" fillId="3" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf fontId="2" fillId="7" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf fontId="2" fillId="8" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf fontId="2" fillId="8" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf fontId="4" fillId="7" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -753,7 +762,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView topLeftCell="F1" zoomScale="100" workbookViewId="0">
+    <sheetView zoomScale="100" workbookViewId="0">
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -866,44 +875,46 @@
       </c>
       <c r="N3" s="1"/>
     </row>
-    <row r="4" ht="14.25">
+    <row r="4" s="8" customFormat="1" ht="14.25">
       <c r="A4" s="8"/>
-      <c r="B4" s="1">
+      <c r="B4" s="8">
         <v>24</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4" s="8">
         <v>20</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D4" s="8">
         <v>200</v>
       </c>
-      <c r="E4" s="1">
+      <c r="E4" s="8">
         <v>10</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="F4" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="G4" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="H4" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="I4" s="1">
-        <v>0</v>
-      </c>
-      <c r="J4" s="9">
-        <v>0</v>
-      </c>
-      <c r="M4" s="1" t="s">
+      <c r="I4" s="8">
+        <v>0</v>
+      </c>
+      <c r="J4" s="8">
+        <v>0</v>
+      </c>
+      <c r="K4" s="8"/>
+      <c r="L4" s="8"/>
+      <c r="M4" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="N4" s="10">
+      <c r="N4" s="8">
         <v>25</v>
       </c>
     </row>
     <row r="5" ht="14.25">
-      <c r="A5" s="8"/>
+      <c r="A5" s="9"/>
       <c r="B5" s="1">
         <v>32</v>
       </c>
@@ -928,7 +939,7 @@
       <c r="I5" s="1">
         <v>0</v>
       </c>
-      <c r="J5" s="9">
+      <c r="J5" s="10">
         <v>0</v>
       </c>
       <c r="M5" s="1" t="s">
@@ -936,7 +947,7 @@
       </c>
     </row>
     <row r="6" ht="14.25">
-      <c r="A6" s="8"/>
+      <c r="A6" s="9"/>
       <c r="B6" s="1">
         <v>48</v>
       </c>
@@ -969,7 +980,7 @@
       </c>
     </row>
     <row r="7" ht="14.25">
-      <c r="A7" s="8"/>
+      <c r="A7" s="9"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
@@ -989,7 +1000,7 @@
       <c r="G8" s="5"/>
     </row>
     <row r="9" ht="14.25">
-      <c r="A9" s="8" t="s">
+      <c r="A9" s="9" t="s">
         <v>21</v>
       </c>
       <c r="B9" s="1">
@@ -1016,57 +1027,57 @@
       <c r="I9" s="1">
         <v>0</v>
       </c>
-      <c r="J9" s="9">
+      <c r="J9" s="10">
         <v>0</v>
       </c>
       <c r="M9" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="10" ht="14.25">
-      <c r="A10" s="8"/>
-      <c r="B10" s="1">
+    <row r="10" s="11" customFormat="1" ht="14.25">
+      <c r="A10" s="11"/>
+      <c r="B10" s="11">
         <v>24</v>
       </c>
-      <c r="C10" s="1">
+      <c r="C10" s="11">
         <v>20</v>
       </c>
-      <c r="D10" s="1">
+      <c r="D10" s="11">
         <v>200</v>
       </c>
-      <c r="E10" s="1">
+      <c r="E10" s="11">
         <v>10</v>
       </c>
-      <c r="F10" s="1" t="s">
+      <c r="F10" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="G10" s="1" t="s">
+      <c r="G10" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="H10" s="1" t="s">
+      <c r="H10" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="I10" s="1">
-        <v>0</v>
-      </c>
-      <c r="J10" s="9">
-        <v>0</v>
-      </c>
-      <c r="K10" s="1" t="s">
+      <c r="I10" s="11">
+        <v>0</v>
+      </c>
+      <c r="J10" s="11">
+        <v>0</v>
+      </c>
+      <c r="K10" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="L10" s="1" t="s">
+      <c r="L10" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="M10" s="1" t="s">
+      <c r="M10" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="N10" s="10">
+      <c r="N10" s="11">
         <v>25</v>
       </c>
     </row>
     <row r="11" ht="14.25">
-      <c r="A11" s="8"/>
+      <c r="A11" s="9"/>
       <c r="B11" s="1">
         <v>32</v>
       </c>
@@ -1091,7 +1102,7 @@
       <c r="I11" s="1">
         <v>0</v>
       </c>
-      <c r="J11" s="9">
+      <c r="J11" s="10">
         <v>0</v>
       </c>
       <c r="M11" s="1" t="s">
@@ -1099,7 +1110,7 @@
       </c>
     </row>
     <row r="12" ht="14.25">
-      <c r="A12" s="8"/>
+      <c r="A12" s="9"/>
       <c r="B12" s="1">
         <v>48</v>
       </c>
@@ -1124,7 +1135,7 @@
       <c r="I12" s="1">
         <v>0</v>
       </c>
-      <c r="J12" s="9">
+      <c r="J12" s="10">
         <v>0</v>
       </c>
       <c r="M12" s="1" t="s">
@@ -1132,7 +1143,7 @@
       </c>
     </row>
     <row r="13" ht="14.25">
-      <c r="A13" s="8"/>
+      <c r="A13" s="9"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
@@ -1141,7 +1152,7 @@
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
-      <c r="J13" s="9"/>
+      <c r="J13" s="10"/>
     </row>
     <row r="14" s="5" customFormat="1" ht="15">
       <c r="A14" s="5" t="s">
@@ -1157,52 +1168,52 @@
       <c r="I14" s="5"/>
       <c r="J14" s="5"/>
     </row>
-    <row r="15" ht="14.25">
+    <row r="15" s="8" customFormat="1" ht="14.25">
       <c r="A15" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="B15" s="1">
+      <c r="B15" s="8">
         <v>96</v>
       </c>
-      <c r="C15" s="1">
+      <c r="C15" s="8">
         <v>20</v>
       </c>
-      <c r="D15" s="1">
+      <c r="D15" s="8">
         <v>100</v>
       </c>
-      <c r="E15" s="1">
+      <c r="E15" s="8">
         <v>40</v>
       </c>
-      <c r="F15" s="1" t="s">
+      <c r="F15" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="G15" s="1" t="s">
+      <c r="G15" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="H15" s="1" t="s">
+      <c r="H15" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="I15" s="1">
-        <v>0</v>
-      </c>
-      <c r="J15" s="9">
-        <v>0</v>
-      </c>
-      <c r="K15" s="1" t="s">
+      <c r="I15" s="8">
+        <v>0</v>
+      </c>
+      <c r="J15" s="8">
+        <v>0</v>
+      </c>
+      <c r="K15" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="L15" s="1" t="s">
+      <c r="L15" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="M15" s="1">
-        <v>0</v>
-      </c>
-      <c r="N15" s="10">
+      <c r="M15" s="8">
+        <v>0</v>
+      </c>
+      <c r="N15" s="8">
         <v>10</v>
       </c>
     </row>
     <row r="16" ht="14.25">
-      <c r="A16" s="8"/>
+      <c r="A16" s="9"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
@@ -1211,7 +1222,7 @@
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
-      <c r="J16" s="9"/>
+      <c r="J16" s="10"/>
     </row>
     <row r="17" s="5" customFormat="1" ht="15">
       <c r="A17" s="5" t="s">
@@ -1221,7 +1232,7 @@
       <c r="F17" s="5"/>
       <c r="G17" s="5"/>
     </row>
-    <row r="18" ht="14.25">
+    <row r="18" s="1" customFormat="1" ht="14.25">
       <c r="A18" s="8" t="s">
         <v>29</v>
       </c>
@@ -1249,57 +1260,60 @@
       <c r="I18" s="1">
         <v>0</v>
       </c>
-      <c r="J18" s="9">
-        <v>0</v>
-      </c>
+      <c r="J18" s="1">
+        <v>0</v>
+      </c>
+      <c r="K18" s="1"/>
+      <c r="L18" s="1"/>
       <c r="M18" s="1">
         <v>0</v>
       </c>
-      <c r="N18" s="10">
+      <c r="N18" s="1"/>
+    </row>
+    <row r="19" s="8" customFormat="1" ht="14.25">
+      <c r="A19" s="8"/>
+      <c r="B19" s="8">
+        <v>120</v>
+      </c>
+      <c r="C19" s="8">
+        <v>20</v>
+      </c>
+      <c r="D19" s="8">
+        <v>75</v>
+      </c>
+      <c r="E19" s="8">
+        <v>54</v>
+      </c>
+      <c r="F19" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="G19" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="H19" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="I19" s="8">
+        <v>0</v>
+      </c>
+      <c r="J19" s="8">
+        <v>0</v>
+      </c>
+      <c r="K19" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="L19" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="M19" s="8">
+        <v>0</v>
+      </c>
+      <c r="N19" s="8">
         <v>10</v>
       </c>
     </row>
-    <row r="19" ht="14.25">
-      <c r="A19" s="8"/>
-      <c r="B19" s="1">
-        <v>120</v>
-      </c>
-      <c r="C19" s="1">
-        <v>20</v>
-      </c>
-      <c r="D19" s="1">
-        <v>75</v>
-      </c>
-      <c r="E19" s="1">
-        <v>54</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="H19" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="I19" s="1">
-        <v>0</v>
-      </c>
-      <c r="J19" s="9">
-        <v>0</v>
-      </c>
-      <c r="K19" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="L19" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="M19" s="1">
-        <v>0</v>
-      </c>
-    </row>
     <row r="20" ht="14.25">
-      <c r="A20" s="8"/>
+      <c r="A20" s="9"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
@@ -1308,10 +1322,10 @@
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
-      <c r="J20" s="9"/>
+      <c r="J20" s="10"/>
     </row>
     <row r="21" ht="14.25">
-      <c r="A21" s="8"/>
+      <c r="A21" s="9"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
@@ -1320,7 +1334,7 @@
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
-      <c r="J21" s="9"/>
+      <c r="J21" s="10"/>
     </row>
     <row r="22" s="5" customFormat="1" ht="15">
       <c r="A22" s="5" t="s">
@@ -1330,7 +1344,7 @@
       <c r="F22" s="5"/>
     </row>
     <row r="23" ht="14.25">
-      <c r="A23" s="8" t="s">
+      <c r="A23" s="9" t="s">
         <v>33</v>
       </c>
     </row>

</xml_diff>

<commit_message>
ven 20 gen 2023, 11:49:05, CET
</commit_message>
<xml_diff>
--- a/simulations.xlsx
+++ b/simulations.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
   <si>
     <t>Machine</t>
   </si>
@@ -57,6 +57,9 @@
     <t xml:space="preserve">sample running per dev</t>
   </si>
   <si>
+    <t xml:space="preserve">must thermalize</t>
+  </si>
+  <si>
     <t>visnu</t>
   </si>
   <si>
@@ -75,6 +78,9 @@
     <t>both</t>
   </si>
   <si>
+    <t>yes</t>
+  </si>
+  <si>
     <t>durga</t>
   </si>
   <si>
@@ -97,6 +103,9 @@
   </si>
   <si>
     <t>251.16</t>
+  </si>
+  <si>
+    <t>no</t>
   </si>
   <si>
     <t>ecaton</t>
@@ -762,7 +771,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView zoomScale="100" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScale="100" workbookViewId="0">
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -779,8 +788,9 @@
     <col customWidth="1" min="11" max="11" style="1" width="21.00390625"/>
     <col customWidth="1" min="12" max="12" style="1" width="13.7109375"/>
     <col customWidth="1" min="13" max="13" style="1" width="18.28125"/>
-    <col customWidth="1" min="14" max="14" style="1" width="27.421875"/>
-    <col min="15" max="16384" style="1" width="9.140625"/>
+    <col customWidth="1" min="14" max="14" style="1" width="29.57421875"/>
+    <col customWidth="1" min="15" max="15" style="1" width="17.8515625"/>
+    <col min="16" max="16384" style="1" width="9.140625"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.25">
@@ -826,10 +836,13 @@
       <c r="N1" s="1" t="s">
         <v>13</v>
       </c>
+      <c r="O1" s="1" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="2" s="5" customFormat="1" ht="14.25">
       <c r="A2" s="6" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B2" s="7"/>
       <c r="C2" s="7"/>
@@ -841,7 +854,7 @@
     </row>
     <row r="3" ht="14.25">
       <c r="A3" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B3" s="1">
         <v>18</v>
@@ -856,13 +869,13 @@
         <v>10</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I3" s="1">
         <v>100</v>
@@ -871,9 +884,12 @@
         <v>0</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="N3" s="1"/>
+      <c r="O3" s="1" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="4" s="8" customFormat="1" ht="14.25">
       <c r="A4" s="8"/>
@@ -890,13 +906,13 @@
         <v>10</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H4" s="8" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I4" s="8">
         <v>0</v>
@@ -907,10 +923,13 @@
       <c r="K4" s="8"/>
       <c r="L4" s="8"/>
       <c r="M4" s="8" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="N4" s="8">
         <v>25</v>
+      </c>
+      <c r="O4" s="8" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="5" ht="14.25">
@@ -928,13 +947,13 @@
         <v>12</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I5" s="1">
         <v>0</v>
@@ -943,7 +962,10 @@
         <v>0</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
+      </c>
+      <c r="O5" s="1" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="6" ht="14.25">
@@ -961,13 +983,13 @@
         <v>14</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I6" s="1">
         <v>0</v>
@@ -976,7 +998,10 @@
         <v>0</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
+      </c>
+      <c r="O6" s="1" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="7" ht="14.25">
@@ -993,7 +1018,7 @@
     </row>
     <row r="8" s="5" customFormat="1" ht="15">
       <c r="A8" s="5" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B8" s="5"/>
       <c r="F8" s="5"/>
@@ -1001,7 +1026,7 @@
     </row>
     <row r="9" ht="14.25">
       <c r="A9" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B9" s="1">
         <v>18</v>
@@ -1016,13 +1041,13 @@
         <v>10</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I9" s="1">
         <v>0</v>
@@ -1031,7 +1056,10 @@
         <v>0</v>
       </c>
       <c r="M9" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
+      </c>
+      <c r="O9" s="1" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="10" s="11" customFormat="1" ht="14.25">
@@ -1049,31 +1077,34 @@
         <v>10</v>
       </c>
       <c r="F10" s="11" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G10" s="11" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H10" s="11" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I10" s="11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J10" s="11">
         <v>0</v>
       </c>
       <c r="K10" s="11" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="L10" s="11" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="M10" s="11" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="N10" s="11">
         <v>25</v>
+      </c>
+      <c r="O10" s="11" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="11" ht="14.25">
@@ -1091,13 +1122,13 @@
         <v>12</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I11" s="1">
         <v>0</v>
@@ -1106,7 +1137,10 @@
         <v>0</v>
       </c>
       <c r="M11" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
+      </c>
+      <c r="O11" s="1" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="12" ht="14.25">
@@ -1124,13 +1158,13 @@
         <v>14</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I12" s="1">
         <v>0</v>
@@ -1139,7 +1173,10 @@
         <v>0</v>
       </c>
       <c r="M12" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
+      </c>
+      <c r="O12" s="1" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="13" ht="14.25">
@@ -1156,7 +1193,7 @@
     </row>
     <row r="14" s="5" customFormat="1" ht="15">
       <c r="A14" s="5" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
@@ -1170,7 +1207,7 @@
     </row>
     <row r="15" s="8" customFormat="1" ht="14.25">
       <c r="A15" s="8" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B15" s="8">
         <v>96</v>
@@ -1185,13 +1222,13 @@
         <v>40</v>
       </c>
       <c r="F15" s="8" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G15" s="8" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H15" s="8" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I15" s="8">
         <v>0</v>
@@ -1200,16 +1237,19 @@
         <v>0</v>
       </c>
       <c r="K15" s="8" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="L15" s="8" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="M15" s="8">
         <v>0</v>
       </c>
       <c r="N15" s="8">
         <v>10</v>
+      </c>
+      <c r="O15" s="8" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="16" ht="14.25">
@@ -1226,7 +1266,7 @@
     </row>
     <row r="17" s="5" customFormat="1" ht="15">
       <c r="A17" s="5" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="B17" s="5"/>
       <c r="F17" s="5"/>
@@ -1234,7 +1274,7 @@
     </row>
     <row r="18" s="1" customFormat="1" ht="14.25">
       <c r="A18" s="8" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="B18" s="1">
         <v>62</v>
@@ -1249,13 +1289,13 @@
         <v>16</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I18" s="1">
         <v>0</v>
@@ -1269,6 +1309,9 @@
         <v>0</v>
       </c>
       <c r="N18" s="1"/>
+      <c r="O18" s="1" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="19" s="8" customFormat="1" ht="14.25">
       <c r="A19" s="8"/>
@@ -1285,13 +1328,13 @@
         <v>54</v>
       </c>
       <c r="F19" s="8" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G19" s="8" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H19" s="8" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I19" s="8">
         <v>0</v>
@@ -1300,10 +1343,10 @@
         <v>0</v>
       </c>
       <c r="K19" s="8" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="L19" s="8" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="M19" s="8">
         <v>0</v>
@@ -1338,14 +1381,14 @@
     </row>
     <row r="22" s="5" customFormat="1" ht="15">
       <c r="A22" s="5" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="B22" s="5"/>
       <c r="F22" s="5"/>
     </row>
     <row r="23" ht="14.25">
       <c r="A23" s="9" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
     </row>
     <row r="25" ht="14.25">

</xml_diff>

<commit_message>
ven 20 gen 2023, 12:33:42, CET
</commit_message>
<xml_diff>
--- a/simulations.xlsx
+++ b/simulations.xlsx
@@ -771,7 +771,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="100" workbookViewId="0">
+    <sheetView topLeftCell="O13" zoomScale="100" workbookViewId="0">
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -1354,6 +1354,9 @@
       <c r="N19" s="8">
         <v>10</v>
       </c>
+      <c r="O19" s="8" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="20" ht="14.25">
       <c r="A20" s="9"/>

</xml_diff>

<commit_message>
Initial commit for KL minimization mar 31 gen 2023, 23:13:55, CET
</commit_message>
<xml_diff>
--- a/simulations.xlsx
+++ b/simulations.xlsx
@@ -771,7 +771,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView topLeftCell="O13" zoomScale="100" workbookViewId="0">
+    <sheetView zoomScale="100" workbookViewId="0">
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -915,7 +915,7 @@
         <v>19</v>
       </c>
       <c r="I4" s="8">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="J4" s="8">
         <v>0</v>
@@ -1086,7 +1086,7 @@
         <v>19</v>
       </c>
       <c r="I10" s="11">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="J10" s="11">
         <v>0</v>

</xml_diff>

<commit_message>
Initial commit for Minimizer_v2.py mer 15 feb 2023, 10:31:00, CET
</commit_message>
<xml_diff>
--- a/simulations.xlsx
+++ b/simulations.xlsx
@@ -771,7 +771,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView zoomScale="100" workbookViewId="0">
+    <sheetView topLeftCell="E10" zoomScale="100" workbookViewId="0">
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -1355,7 +1355,7 @@
         <v>10</v>
       </c>
       <c r="O19" s="8" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
     </row>
     <row r="20" ht="14.25">

</xml_diff>

<commit_message>
mer 8 mar 2023, 16:57:30, CET
</commit_message>
<xml_diff>
--- a/simulations.xlsx
+++ b/simulations.xlsx
@@ -132,36 +132,36 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="5">
     <font>
+      <sz val="11.000000"/>
+      <color theme="1"/>
       <name val="Calibri"/>
-      <color theme="1"/>
-      <sz val="11.000000"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11.000000"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
-      <color rgb="FF9C0006"/>
-      <sz val="11.000000"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11.000000"/>
+      <color theme="1"/>
       <name val="Calibri"/>
-      <b/>
-      <color theme="1"/>
-      <sz val="11.000000"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <name val="Calibri"/>
       <b/>
       <i/>
+      <sz val="11.000000"/>
       <color theme="1"/>
-      <sz val="11.000000"/>
+      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <name val="Calibri"/>
       <b/>
       <sz val="11.000000"/>
+      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -228,7 +228,7 @@
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf fontId="1" fillId="2" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="2" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -261,6 +261,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf fontId="4" fillId="7" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf fontId="1" fillId="2" borderId="0" numFmtId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -771,7 +774,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView topLeftCell="E10" zoomScale="100" workbookViewId="0">
+    <sheetView zoomScale="100" workbookViewId="0">
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -915,7 +918,7 @@
         <v>19</v>
       </c>
       <c r="I4" s="8">
-        <v>30</v>
+        <v>100</v>
       </c>
       <c r="J4" s="8">
         <v>0</v>
@@ -925,9 +928,7 @@
       <c r="M4" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="N4" s="8">
-        <v>25</v>
-      </c>
+      <c r="N4" s="8"/>
       <c r="O4" s="8" t="s">
         <v>21</v>
       </c>
@@ -963,6 +964,9 @@
       </c>
       <c r="M5" s="1" t="s">
         <v>20</v>
+      </c>
+      <c r="N5" s="1">
+        <v>4</v>
       </c>
       <c r="O5" s="1" t="s">
         <v>21</v>
@@ -1086,7 +1090,7 @@
         <v>19</v>
       </c>
       <c r="I10" s="11">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="J10" s="11">
         <v>0</v>
@@ -1245,8 +1249,8 @@
       <c r="M15" s="8">
         <v>0</v>
       </c>
-      <c r="N15" s="8">
-        <v>10</v>
+      <c r="N15" s="12">
+        <v>0</v>
       </c>
       <c r="O15" s="8" t="s">
         <v>30</v>
@@ -1308,53 +1312,55 @@
       <c r="M18" s="1">
         <v>0</v>
       </c>
-      <c r="N18" s="1"/>
+      <c r="N18" s="1">
+        <v>4</v>
+      </c>
       <c r="O18" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="19" s="8" customFormat="1" ht="14.25">
-      <c r="A19" s="8"/>
-      <c r="B19" s="8">
+    <row r="19" s="9" customFormat="1" ht="14.25">
+      <c r="A19" s="9"/>
+      <c r="B19" s="9">
         <v>120</v>
       </c>
-      <c r="C19" s="8">
-        <v>20</v>
-      </c>
-      <c r="D19" s="8">
+      <c r="C19" s="9">
+        <v>20</v>
+      </c>
+      <c r="D19" s="9">
         <v>75</v>
       </c>
-      <c r="E19" s="8">
+      <c r="E19" s="9">
         <v>54</v>
       </c>
-      <c r="F19" s="8" t="s">
+      <c r="F19" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="G19" s="8" t="s">
+      <c r="G19" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="H19" s="8" t="s">
+      <c r="H19" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="I19" s="8">
-        <v>0</v>
-      </c>
-      <c r="J19" s="8">
-        <v>0</v>
-      </c>
-      <c r="K19" s="8" t="s">
+      <c r="I19" s="9">
+        <v>0</v>
+      </c>
+      <c r="J19" s="9">
+        <v>0</v>
+      </c>
+      <c r="K19" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="L19" s="8" t="s">
+      <c r="L19" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="M19" s="8">
-        <v>0</v>
-      </c>
-      <c r="N19" s="8">
+      <c r="M19" s="9">
+        <v>0</v>
+      </c>
+      <c r="N19" s="9">
         <v>10</v>
       </c>
-      <c r="O19" s="8" t="s">
+      <c r="O19" s="9" t="s">
         <v>30</v>
       </c>
     </row>
@@ -1406,7 +1412,7 @@
   </sheetData>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="2147483648" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
   <headerFooter/>
 </worksheet>
 </file>
</xml_diff>